<commit_message>
6 test cases passed
</commit_message>
<xml_diff>
--- a/com.apartments/src/test/resources/test_data_apartments.xlsx
+++ b/com.apartments/src/test/resources/test_data_apartments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.apartments/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7808D3-7371-1640-9F5C-3DF2738693E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635CD140-3FD6-6249-B4C2-2E8B0DB5E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="5" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
@@ -41,14 +41,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Manhattan, NY</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Queens, NY</t>
   </si>
   <si>
@@ -76,26 +73,20 @@
     <t>20000</t>
   </si>
   <si>
-    <t>560-562 W 174th St</t>
+    <t>3k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Menlo"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -123,12 +114,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,18 +435,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2812B8E5-96A4-7B44-BC0F-543C6D645201}">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -480,10 +475,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -505,11 +500,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -529,10 +524,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -558,16 +553,16 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -579,29 +574,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7716E5A1-F4D7-4846-BE85-B3D749139871}">
   <dimension ref="A2:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test case 7 commented and test case 8 passed
</commit_message>
<xml_diff>
--- a/com.apartments/src/test/resources/test_data_apartments.xlsx
+++ b/com.apartments/src/test/resources/test_data_apartments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.apartments/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635CD140-3FD6-6249-B4C2-2E8B0DB5E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC9403B-C422-F14B-A751-21D2B0586643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="7" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="OneFavorite" sheetId="4" r:id="rId4"/>
     <sheet name="WriteAReview" sheetId="5" r:id="rId5"/>
     <sheet name="RentCalculator" sheetId="6" r:id="rId6"/>
+    <sheet name="Authentication" sheetId="7" r:id="rId7"/>
+    <sheet name="ChangeLanguage" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Manhattan, NY</t>
   </si>
@@ -74,13 +76,25 @@
   </si>
   <si>
     <t>3k</t>
+  </si>
+  <si>
+    <t>adilkhaleque429@gmail.com</t>
+  </si>
+  <si>
+    <t>Testunbound6A</t>
+  </si>
+  <si>
+    <t>Adil</t>
+  </si>
+  <si>
+    <t>Español</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,6 +106,14 @@
       <sz val="11"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,16 +133,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,7 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2812B8E5-96A4-7B44-BC0F-543C6D645201}">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -604,4 +629,61 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6EBF3F0-D925-0245-A677-2DFA40113E89}">
+  <dimension ref="A2:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{157D0AF3-9A63-7049-BD61-F72F0361501B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBD47A0-4B58-824C-A1CE-CD1443EBBB34}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test case 9 commented
</commit_message>
<xml_diff>
--- a/com.apartments/src/test/resources/test_data_apartments.xlsx
+++ b/com.apartments/src/test/resources/test_data_apartments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.apartments/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC9403B-C422-F14B-A751-21D2B0586643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8167B991-4007-B946-BAF3-D2B79380DFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="7" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="8" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="RentCalculator" sheetId="6" r:id="rId6"/>
     <sheet name="Authentication" sheetId="7" r:id="rId7"/>
     <sheet name="ChangeLanguage" sheetId="8" r:id="rId8"/>
+    <sheet name="HomesForRent" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Manhattan, NY</t>
   </si>
@@ -88,13 +89,22 @@
   </si>
   <si>
     <t>Español</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homes for Rent in Los Angeles, CA </t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Homes for Rent in Manhattan, NY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,6 +121,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,12 +153,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,13 +478,13 @@
   <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.5" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -475,8 +492,8 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -669,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBD47A0-4B58-824C-A1CE-CD1443EBBB34}">
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -686,4 +703,34 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F95D8D-06F2-1A46-9AB4-BD6345F0BA18}">
+  <dimension ref="A2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="46.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test cases 8, 9, 10 passed
</commit_message>
<xml_diff>
--- a/com.apartments/src/test/resources/test_data_apartments.xlsx
+++ b/com.apartments/src/test/resources/test_data_apartments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.apartments/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F47EA8-06F5-BC43-B2CB-121086413AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14131F0F-15DF-B442-A8C9-24FC11B7BC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="8" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Manhattan, NY</t>
   </si>
@@ -91,13 +91,25 @@
     <t>Español</t>
   </si>
   <si>
-    <t xml:space="preserve">Homes for Rent in Los Angeles, CA </t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
     <t>Homes for Rent in Manhattan, NY</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Homes for Rent in Los Angeles, CA</t>
+  </si>
+  <si>
+    <t>Homes for Rent in Nashville, TN</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Homes for Rent in Phoenix, AZ</t>
   </si>
 </sst>
 </file>
@@ -486,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -700,24 +712,42 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1A6B221-0E2D-6A4F-8FBD-6692BA84E4D9}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="41.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="41.83203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test case 14 passed
</commit_message>
<xml_diff>
--- a/com.apartments/src/test/resources/test_data_apartments.xlsx
+++ b/com.apartments/src/test/resources/test_data_apartments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.apartments/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14131F0F-15DF-B442-A8C9-24FC11B7BC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDDCCB4-E310-B048-A715-4B41C3965642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="8" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" firstSheet="3" activeTab="12" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,11 @@
     <sheet name="RentCalculator" sheetId="6" r:id="rId6"/>
     <sheet name="Authentication" sheetId="7" r:id="rId7"/>
     <sheet name="ChangeLanguage" sheetId="8" r:id="rId8"/>
-    <sheet name="LAHomesForRent" sheetId="10" r:id="rId9"/>
+    <sheet name="HomesForRent" sheetId="10" r:id="rId9"/>
+    <sheet name="ApartmentsForRent" sheetId="11" r:id="rId10"/>
+    <sheet name="CondosForRent" sheetId="12" r:id="rId11"/>
+    <sheet name="TownhomesForRent" sheetId="13" r:id="rId12"/>
+    <sheet name="SavedSearch" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Manhattan, NY</t>
   </si>
@@ -110,6 +114,21 @@
   </si>
   <si>
     <t>Homes for Rent in Phoenix, AZ</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Apartments for Rent in Seattle, WA</t>
+  </si>
+  <si>
+    <t>Condos for Rent in Chicago, IL</t>
+  </si>
+  <si>
+    <t>Townhomes for Rent in Houston, TX</t>
+  </si>
+  <si>
+    <t>&lt; $5,400, Apartments, Luxury, 5 Star Rating</t>
   </si>
 </sst>
 </file>
@@ -506,6 +525,124 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C7B5398-B6C5-754B-84D4-7912E00A0F93}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58666C7F-1425-C044-8942-F1170E02C55F}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A4E353-9CD9-ED4E-9B21-309251AA63F4}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="42.5" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B64D20F9-CFFF-1B4E-B7AD-E66695114B95}">
+  <dimension ref="A2:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="52.6640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{A5E2157B-62B4-6446-BB15-492FA8E31DA5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7ADF543-C6CE-0A4C-9DCF-2C13A79E6F0D}">
   <dimension ref="A2:B2"/>
@@ -658,7 +795,7 @@
   <dimension ref="A2:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,7 +851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1A6B221-0E2D-6A4F-8FBD-6692BA84E4D9}">
   <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
passed all 19 test cases
</commit_message>
<xml_diff>
--- a/com.apartments/src/test/resources/test_data_apartments.xlsx
+++ b/com.apartments/src/test/resources/test_data_apartments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adil/IdeaProjects/SeleniumBootcamp/com.apartments/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C697851-C24B-C94D-92C5-DBEEF941C86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620110A6-D70D-E749-AA01-3D886347112F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" firstSheet="8" activeTab="16" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{21AFA41A-4244-444C-A152-0A848FA08C37}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>Homes for Rent in Manhattan, NY</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>Campuses</t>
+  </si>
+  <si>
+    <t>Apartments for Rent in Manhattan, NY</t>
   </si>
 </sst>
 </file>
@@ -517,14 +517,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2812B8E5-96A4-7B44-BC0F-543C6D645201}">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="40.5" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -556,10 +556,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +585,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -610,10 +610,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +648,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -731,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2567D30-E96F-9D46-953A-C0055D74A08D}">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -986,10 +986,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -997,16 +997,16 @@
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>21</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>